<commit_message>
added 'gg' to 'moving around' tab
</commit_message>
<xml_diff>
--- a/vimMastery.xlsx
+++ b/vimMastery.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueorigins-my.sharepoint.us/personal/thoyle_blueorigin_com/Documents/cmd spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{14C54E62-9728-4DC7-8A9A-DAB4372A8B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3B0EACA-026C-446F-AB3B-CB9C5EB0D6B4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3AFF2BC-1942-4D7B-8284-99C9A702FE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{2B2C4A5C-E235-4775-ABF4-D4C44A5B2836}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2B2C4A5C-E235-4775-ABF4-D4C44A5B2836}"/>
   </bookViews>
   <sheets>
     <sheet name="quick guide" sheetId="17" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="645">
   <si>
     <t>VIM GENERAL NOTES</t>
   </si>
@@ -15497,6 +15497,35 @@
     <t xml:space="preserve">selects lines 33 - 42 of a file, then deletes the first character on each of those lines
 :33,42 = select lines 33 - 42
 </t>
+  </si>
+  <si>
+    <t>FILE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = move to beginning of file</t>
+    </r>
+  </si>
+  <si>
+    <t>moves cursor to the beginning of the first line in a file</t>
   </si>
 </sst>
 </file>
@@ -15583,7 +15612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -15692,14 +15721,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -16027,23 +16065,23 @@
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="28"/>
-    <col min="2" max="2" width="38.36328125" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="38.08984375" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.08984375" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="28"/>
+    <col min="1" max="1" width="8.85546875" style="28"/>
+    <col min="2" max="2" width="38.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="2:5" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
         <v>563</v>
       </c>
@@ -16052,7 +16090,7 @@
       </c>
       <c r="E2" s="35"/>
     </row>
-    <row r="3" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="36" t="s">
         <v>553</v>
       </c>
@@ -16062,7 +16100,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="32" t="s">
         <v>178</v>
       </c>
@@ -16074,7 +16112,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>538</v>
       </c>
@@ -16084,7 +16122,7 @@
       </c>
       <c r="E5" s="26"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>218</v>
       </c>
@@ -16094,7 +16132,7 @@
       </c>
       <c r="E6" s="26"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>539</v>
       </c>
@@ -16106,7 +16144,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>546</v>
       </c>
@@ -16118,7 +16156,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>540</v>
       </c>
@@ -16127,7 +16165,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>333</v>
       </c>
@@ -16137,7 +16175,7 @@
       </c>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>626</v>
       </c>
@@ -16146,7 +16184,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
         <v>627</v>
       </c>
@@ -16155,7 +16193,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>572</v>
       </c>
@@ -16167,7 +16205,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="28" t="s">
@@ -16177,13 +16215,13 @@
         <v>558</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="28" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>548</v>
       </c>
@@ -16192,18 +16230,18 @@
         <v>556</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>
       <c r="D17" s="33" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D18" s="33" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D19" s="33" t="s">
         <v>547</v>
       </c>
@@ -16211,15 +16249,15 @@
         <v>564</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D23" s="9" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D24" s="33" t="s">
         <v>554</v>
       </c>
@@ -16227,7 +16265,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D25" s="28" t="s">
         <v>547</v>
       </c>
@@ -16235,22 +16273,22 @@
         <v>560</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="D26" s="25" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="28" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="28" t="s">
         <v>566</v>
       </c>
@@ -16273,21 +16311,21 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="28"/>
-    <col min="2" max="2" width="32.6328125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="28.6328125" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" style="28" customWidth="1"/>
-    <col min="5" max="16384" width="8.90625" style="28"/>
+    <col min="1" max="1" width="8.85546875" style="28"/>
+    <col min="2" max="2" width="32.5703125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
         <v>484</v>
       </c>
@@ -16296,7 +16334,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>502</v>
       </c>
@@ -16305,7 +16343,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
         <v>499</v>
       </c>
@@ -16316,7 +16354,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>503</v>
       </c>
@@ -16327,7 +16365,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="180" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>505</v>
       </c>
@@ -16338,7 +16376,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="101" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="101.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>508</v>
       </c>
@@ -16366,21 +16404,21 @@
       <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="28"/>
+    <col min="1" max="1" width="8.85546875" style="28"/>
     <col min="2" max="2" width="33" style="28" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" style="28" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" style="28" customWidth="1"/>
-    <col min="5" max="16384" width="8.90625" style="28"/>
+    <col min="3" max="3" width="27.5703125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
         <v>484</v>
       </c>
@@ -16389,7 +16427,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>485</v>
       </c>
@@ -16398,7 +16436,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
         <v>487</v>
       </c>
@@ -16409,7 +16447,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="86.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>489</v>
       </c>
@@ -16420,7 +16458,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="145" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="165" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>490</v>
       </c>
@@ -16431,7 +16469,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>498</v>
       </c>
@@ -16460,20 +16498,20 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
-    <col min="5" max="5" width="43.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
+    <col min="5" max="5" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="73.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -16482,7 +16520,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="36" t="s">
         <v>444</v>
       </c>
@@ -16492,7 +16530,7 @@
       </c>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>445</v>
       </c>
@@ -16506,7 +16544,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
         <v>448</v>
       </c>
@@ -16518,7 +16556,7 @@
       </c>
       <c r="E5" s="35"/>
     </row>
-    <row r="6" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>451</v>
       </c>
@@ -16530,7 +16568,7 @@
       </c>
       <c r="E6" s="35"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>454</v>
       </c>
@@ -16542,7 +16580,7 @@
       </c>
       <c r="E7" s="35"/>
     </row>
-    <row r="8" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>457</v>
       </c>
@@ -16554,7 +16592,7 @@
       </c>
       <c r="E8" s="35"/>
     </row>
-    <row r="9" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>460</v>
       </c>
@@ -16566,7 +16604,7 @@
       </c>
       <c r="E9" s="35"/>
     </row>
-    <row r="10" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="31" t="s">
         <v>463</v>
       </c>
@@ -16578,7 +16616,7 @@
       </c>
       <c r="E10" s="14"/>
     </row>
-    <row r="11" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>466</v>
       </c>
@@ -16590,7 +16628,7 @@
       </c>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>469</v>
       </c>
@@ -16602,7 +16640,7 @@
       </c>
       <c r="E12" s="13"/>
     </row>
-    <row r="13" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
         <v>472</v>
       </c>
@@ -16633,19 +16671,19 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="73.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="73.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -16654,14 +16692,14 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>38</v>
       </c>
@@ -16670,12 +16708,12 @@
       </c>
       <c r="D4" s="35"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="11"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="36" t="s">
         <v>355</v>
       </c>
@@ -16684,7 +16722,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="203" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="210" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>477</v>
       </c>
@@ -16695,7 +16733,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
         <v>482</v>
       </c>
@@ -16725,19 +16763,19 @@
       <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="73.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="73.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -16746,7 +16784,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>410</v>
       </c>
@@ -16755,7 +16793,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>411</v>
       </c>
@@ -16766,7 +16804,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>414</v>
       </c>
@@ -16777,7 +16815,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>417</v>
       </c>
@@ -16788,7 +16826,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>420</v>
       </c>
@@ -16799,7 +16837,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>423</v>
       </c>
@@ -16827,19 +16865,19 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -16848,12 +16886,12 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="2:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>385</v>
       </c>
@@ -16862,7 +16900,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>386</v>
       </c>
@@ -16873,7 +16911,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>389</v>
       </c>
@@ -16884,7 +16922,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>392</v>
       </c>
@@ -16895,7 +16933,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>395</v>
       </c>
@@ -16906,7 +16944,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
         <v>398</v>
       </c>
@@ -16917,7 +16955,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
         <v>401</v>
       </c>
@@ -16928,7 +16966,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>629</v>
       </c>
@@ -16939,7 +16977,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C15" s="31"/>
     </row>
   </sheetData>
@@ -16959,19 +16997,19 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:4" s="11" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" s="11" customFormat="1" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -16980,7 +17018,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>29</v>
       </c>
@@ -16989,7 +17027,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
@@ -17000,7 +17038,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>325</v>
       </c>
@@ -17011,7 +17049,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>318</v>
       </c>
@@ -17019,7 +17057,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>323</v>
       </c>
@@ -17027,7 +17065,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>349</v>
       </c>
@@ -17056,22 +17094,22 @@
       <selection activeCell="U49" sqref="U49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.08984375" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="41" t="s">
+    <row r="3" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="41"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="35" t="s">
         <v>39</v>
       </c>
@@ -17081,9 +17119,9 @@
       <c r="H3" s="35"/>
       <c r="I3" s="35"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
       <c r="F4" s="35"/>
@@ -17091,9 +17129,9 @@
       <c r="H4" s="35"/>
       <c r="I4" s="35"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
       <c r="F5" s="35"/>
@@ -17101,9 +17139,9 @@
       <c r="H5" s="35"/>
       <c r="I5" s="35"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="35"/>
       <c r="E6" s="35"/>
       <c r="F6" s="35"/>
@@ -17111,20 +17149,20 @@
       <c r="H6" s="35"/>
       <c r="I6" s="35"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="9" spans="2:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="42" t="s">
+    <row r="9" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-    </row>
-    <row r="11" spans="2:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+    </row>
+    <row r="11" spans="2:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="35" t="s">
         <v>1</v>
       </c>
@@ -17138,7 +17176,7 @@
       <c r="J11" s="35"/>
       <c r="K11" s="35"/>
     </row>
-    <row r="12" spans="2:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="35" t="s">
         <v>2</v>
       </c>
@@ -17152,7 +17190,7 @@
       <c r="J12" s="35"/>
       <c r="K12" s="35"/>
     </row>
-    <row r="13" spans="2:11" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="35" t="s">
         <v>3</v>
       </c>
@@ -17166,21 +17204,21 @@
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B14" s="41" t="s">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-    </row>
-    <row r="15" spans="2:11" ht="116.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+    </row>
+    <row r="15" spans="2:11" ht="116.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="35" t="s">
         <v>5</v>
       </c>
@@ -17194,7 +17232,7 @@
       <c r="J15" s="35"/>
       <c r="K15" s="35"/>
     </row>
-    <row r="16" spans="2:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="35" t="s">
         <v>623</v>
       </c>
@@ -17210,13 +17248,13 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="42" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="42"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="45"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
@@ -17224,7 +17262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
         <v>9</v>
       </c>
@@ -17232,7 +17270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
         <v>11</v>
       </c>
@@ -17240,7 +17278,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
         <v>13</v>
       </c>
@@ -17248,7 +17286,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
@@ -17256,7 +17294,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
@@ -17264,16 +17302,16 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="41" t="s">
+      <c r="D24" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="41"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E24" s="44"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
         <v>17</v>
       </c>
@@ -17281,7 +17319,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
         <v>18</v>
       </c>
@@ -17289,7 +17327,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" s="4" t="s">
         <v>20</v>
       </c>
@@ -17297,7 +17335,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
         <v>19</v>
       </c>
@@ -17305,230 +17343,230 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="41" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="44" t="s">
         <v>512</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="41" t="s">
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="44" t="s">
         <v>513</v>
       </c>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="41" t="s">
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="44" t="s">
         <v>514</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="41" t="s">
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="44" t="s">
         <v>515</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="41" t="s">
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="44" t="s">
         <v>516</v>
       </c>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="41" t="s">
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="44" t="s">
         <v>517</v>
       </c>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="41" t="s">
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="44" t="s">
         <v>518</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="41" t="s">
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="44" t="s">
         <v>519</v>
       </c>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B38" s="44"/>
+      <c r="C38" s="44"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="35" t="s">
         <v>520</v>
       </c>
       <c r="B39" s="35"/>
       <c r="C39" s="35"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
         <v>521</v>
       </c>
       <c r="B40" s="35"/>
       <c r="C40" s="35"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="41" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="44" t="s">
         <v>522</v>
       </c>
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="41" t="s">
+      <c r="B41" s="44"/>
+      <c r="C41" s="44"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="44" t="s">
         <v>523</v>
       </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>524</v>
       </c>
       <c r="B43" s="28"/>
       <c r="C43" s="28"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
         <v>525</v>
       </c>
       <c r="B44" s="28"/>
       <c r="C44" s="28"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
         <v>526</v>
       </c>
       <c r="B45" s="28"/>
       <c r="C45" s="28"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>527</v>
       </c>
       <c r="B46" s="28"/>
       <c r="C46" s="28"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
         <v>528</v>
       </c>
       <c r="B47" s="28"/>
       <c r="C47" s="28"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
         <v>529</v>
       </c>
       <c r="B48" s="28"/>
       <c r="C48" s="28"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
         <v>530</v>
       </c>
       <c r="B49" s="28"/>
       <c r="C49" s="28"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>531</v>
       </c>
       <c r="B50" s="28"/>
       <c r="C50" s="28"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>532</v>
       </c>
       <c r="B51" s="28"/>
       <c r="C51" s="28"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
         <v>533</v>
       </c>
       <c r="B52" s="28"/>
       <c r="C52" s="28"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>534</v>
       </c>
       <c r="B53" s="28"/>
       <c r="C53" s="28"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>535</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>536</v>
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>573</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>598</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>537</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>567</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>625</v>
       </c>
@@ -17573,21 +17611,21 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="28"/>
-    <col min="2" max="2" width="31.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.6328125" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" style="28" customWidth="1"/>
-    <col min="5" max="16384" width="9.08984375" style="28"/>
+    <col min="1" max="1" width="9.140625" style="28"/>
+    <col min="2" max="2" width="31.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>38</v>
       </c>
@@ -17596,7 +17634,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>633</v>
       </c>
@@ -17604,7 +17642,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>634</v>
       </c>
@@ -17628,19 +17666,19 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -17649,7 +17687,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>40</v>
       </c>
@@ -17658,7 +17696,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>41</v>
       </c>
@@ -17669,7 +17707,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>44</v>
       </c>
@@ -17680,7 +17718,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>47</v>
       </c>
@@ -17691,7 +17729,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>50</v>
       </c>
@@ -17702,7 +17740,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>53</v>
       </c>
@@ -17713,7 +17751,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>56</v>
       </c>
@@ -17724,7 +17762,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>59</v>
       </c>
@@ -17735,7 +17773,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>62</v>
       </c>
@@ -17746,7 +17784,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
         <v>65</v>
       </c>
@@ -17757,7 +17795,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>68</v>
       </c>
@@ -17768,7 +17806,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
         <v>71</v>
       </c>
@@ -17779,7 +17817,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
         <v>74</v>
       </c>
@@ -17790,7 +17828,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
         <v>77</v>
       </c>
@@ -17818,20 +17856,20 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
-    <col min="5" max="5" width="48.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -17840,7 +17878,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>97</v>
       </c>
@@ -17850,7 +17888,7 @@
       </c>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>98</v>
       </c>
@@ -17864,7 +17902,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>102</v>
       </c>
@@ -17876,7 +17914,7 @@
       </c>
       <c r="E6" s="37"/>
     </row>
-    <row r="7" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>105</v>
       </c>
@@ -17900,26 +17938,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA205936-45F5-47FC-ABEA-5B92E2F781D2}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
-    <col min="5" max="5" width="39.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -17928,7 +17966,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>108</v>
       </c>
@@ -17938,8 +17976,8 @@
       </c>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
         <v>245</v>
       </c>
       <c r="B5" s="16"/>
@@ -17947,8 +17985,8 @@
       <c r="D5" s="19"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="39"/>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="40"/>
       <c r="B6" s="22" t="s">
         <v>130</v>
       </c>
@@ -17960,8 +17998,8 @@
       </c>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="39"/>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="40"/>
       <c r="B7" s="22" t="s">
         <v>133</v>
       </c>
@@ -17973,8 +18011,8 @@
       </c>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="39"/>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="40"/>
       <c r="B8" s="22" t="s">
         <v>136</v>
       </c>
@@ -17986,8 +18024,8 @@
       </c>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="39"/>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="40"/>
       <c r="B9" s="22" t="s">
         <v>139</v>
       </c>
@@ -17999,19 +18037,19 @@
       </c>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="39"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="10"/>
       <c r="D11" s="7"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="38" t="s">
+    <row r="12" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
         <v>176</v>
       </c>
       <c r="B12" s="22" t="s">
@@ -18023,12 +18061,12 @@
       <c r="D12" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="41" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="38"/>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
       <c r="B13" s="22" t="s">
         <v>144</v>
       </c>
@@ -18038,10 +18076,10 @@
       <c r="D13" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="40"/>
-    </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="38"/>
+      <c r="E13" s="41"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="39"/>
       <c r="B14" s="22" t="s">
         <v>147</v>
       </c>
@@ -18051,10 +18089,10 @@
       <c r="D14" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E14" s="40"/>
-    </row>
-    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="38"/>
+      <c r="E14" s="41"/>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="39"/>
       <c r="B15" s="22" t="s">
         <v>150</v>
       </c>
@@ -18064,10 +18102,10 @@
       <c r="D15" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="E15" s="40"/>
-    </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="38"/>
+      <c r="E15" s="41"/>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="39"/>
       <c r="B16" s="22" t="s">
         <v>153</v>
       </c>
@@ -18079,8 +18117,8 @@
       </c>
       <c r="E16" s="20"/>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="38"/>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
       <c r="B17" s="22" t="s">
         <v>156</v>
       </c>
@@ -18092,8 +18130,8 @@
       </c>
       <c r="E17" s="20"/>
     </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="38"/>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="39"/>
       <c r="B18" s="22" t="s">
         <v>192</v>
       </c>
@@ -18105,8 +18143,8 @@
       </c>
       <c r="E18" s="20"/>
     </row>
-    <row r="19" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="38"/>
+    <row r="19" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="39"/>
       <c r="B19" s="22" t="s">
         <v>193</v>
       </c>
@@ -18118,8 +18156,8 @@
       </c>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="38"/>
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="39"/>
       <c r="B20" s="22" t="s">
         <v>595</v>
       </c>
@@ -18131,15 +18169,15 @@
       </c>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
       <c r="C21" s="10"/>
       <c r="D21" s="8"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="39" t="s">
+    <row r="22" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="40" t="s">
         <v>175</v>
       </c>
       <c r="B22" s="23" t="s">
@@ -18153,8 +18191,8 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="39"/>
+    <row r="23" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="40"/>
       <c r="B23" s="22" t="s">
         <v>261</v>
       </c>
@@ -18166,8 +18204,8 @@
       </c>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="39"/>
+    <row r="24" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="40"/>
       <c r="B24" s="22" t="s">
         <v>161</v>
       </c>
@@ -18179,8 +18217,8 @@
       </c>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="39"/>
+    <row r="25" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="40"/>
       <c r="B25" s="16" t="s">
         <v>164</v>
       </c>
@@ -18192,8 +18230,8 @@
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="39"/>
+    <row r="26" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="40"/>
       <c r="B26" s="16" t="s">
         <v>266</v>
       </c>
@@ -18205,8 +18243,8 @@
       </c>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="39"/>
+    <row r="27" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="40"/>
       <c r="B27" s="16" t="s">
         <v>260</v>
       </c>
@@ -18218,15 +18256,15 @@
       </c>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="10"/>
       <c r="D28" s="8"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:5" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="38" t="s">
+    <row r="29" spans="1:5" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
         <v>258</v>
       </c>
       <c r="B29" s="22" t="s">
@@ -18240,8 +18278,8 @@
       </c>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A30" s="38"/>
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="39"/>
       <c r="B30" s="22" t="s">
         <v>253</v>
       </c>
@@ -18253,15 +18291,15 @@
       </c>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="22"/>
       <c r="C31" s="10"/>
       <c r="D31" s="8"/>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="39" t="s">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="40" t="s">
         <v>259</v>
       </c>
       <c r="B32" s="22" t="s">
@@ -18275,8 +18313,8 @@
       </c>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="39"/>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="40"/>
       <c r="B33" s="22" t="s">
         <v>123</v>
       </c>
@@ -18288,11 +18326,11 @@
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E34" s="11"/>
     </row>
-    <row r="35" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="38" t="s">
+    <row r="35" spans="1:5" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="39" t="s">
         <v>174</v>
       </c>
       <c r="B35" s="22" t="s">
@@ -18306,8 +18344,8 @@
       </c>
       <c r="E35" s="11"/>
     </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="38"/>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="39"/>
       <c r="B36" s="22" t="s">
         <v>112</v>
       </c>
@@ -18319,8 +18357,8 @@
       </c>
       <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="38"/>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="39"/>
       <c r="B37" s="22" t="s">
         <v>115</v>
       </c>
@@ -18331,8 +18369,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="38"/>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="39"/>
       <c r="B38" s="9" t="s">
         <v>118</v>
       </c>
@@ -18343,8 +18381,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="38"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="39"/>
       <c r="B39" s="22" t="s">
         <v>125</v>
       </c>
@@ -18355,8 +18393,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="38"/>
+    <row r="40" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="39"/>
       <c r="B40" s="22" t="s">
         <v>128</v>
       </c>
@@ -18367,8 +18405,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="38"/>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="39"/>
       <c r="B41" s="22" t="s">
         <v>273</v>
       </c>
@@ -18379,8 +18417,8 @@
         <v>274</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="38"/>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="39"/>
       <c r="B42" s="16" t="s">
         <v>171</v>
       </c>
@@ -18391,8 +18429,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="38"/>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="39"/>
       <c r="B43" s="16" t="s">
         <v>316</v>
       </c>
@@ -18403,8 +18441,8 @@
         <v>317</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="38"/>
+    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="39"/>
       <c r="B44" s="15" t="s">
         <v>344</v>
       </c>
@@ -18415,8 +18453,8 @@
         <v>346</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="38"/>
+    <row r="45" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="39"/>
       <c r="B45" s="15" t="s">
         <v>345</v>
       </c>
@@ -18427,43 +18465,94 @@
         <v>347</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="9"/>
       <c r="D46" s="14"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B47" s="16" t="s">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="38" t="s">
+        <v>642</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>643</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="38"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="14"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="38"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="14"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="38"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="14"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="38"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="14"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="14"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="14"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="16" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B48" s="16" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="16" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="16" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="16" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="16" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="16" t="s">
         <v>265</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A35:A45"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B4:C4"/>
+  <mergeCells count="10">
     <mergeCell ref="E12:E15"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A35:A45"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18478,20 +18567,20 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
-    <col min="5" max="5" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:5" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -18500,7 +18589,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>180</v>
       </c>
@@ -18509,7 +18598,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>320</v>
       </c>
@@ -18520,7 +18609,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>182</v>
       </c>
@@ -18531,7 +18620,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
         <v>184</v>
       </c>
@@ -18542,7 +18631,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>322</v>
       </c>
@@ -18553,7 +18642,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>602</v>
       </c>
@@ -18564,7 +18653,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
         <v>188</v>
       </c>
@@ -18575,7 +18664,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>605</v>
       </c>
@@ -18586,7 +18675,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
         <v>606</v>
       </c>
@@ -18597,7 +18686,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
         <v>609</v>
       </c>
@@ -18608,12 +18697,12 @@
         <v>611</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="22"/>
       <c r="C14" s="10"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="36" t="s">
         <v>612</v>
       </c>
@@ -18622,7 +18711,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:5" s="31" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" s="31" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
         <v>361</v>
       </c>
@@ -18634,7 +18723,7 @@
       </c>
       <c r="E16" s="33"/>
     </row>
-    <row r="17" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="29" t="s">
         <v>363</v>
       </c>
@@ -18645,7 +18734,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
         <v>366</v>
       </c>
@@ -18656,7 +18745,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>622</v>
       </c>
@@ -18664,7 +18753,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>637</v>
       </c>
@@ -18690,23 +18779,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C5EEE4-9C59-4B4E-BDC3-2865A323AE75}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -18715,7 +18804,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>199</v>
       </c>
@@ -18724,8 +18813,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="38" t="s">
+    <row r="5" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
         <v>245</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -18738,8 +18827,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="38"/>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="43"/>
       <c r="B6" s="13" t="s">
         <v>203</v>
       </c>
@@ -18750,8 +18839,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="38"/>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="43"/>
       <c r="B7" s="25" t="s">
         <v>206</v>
       </c>
@@ -18762,8 +18851,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="38"/>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="43"/>
       <c r="B8" s="16" t="s">
         <v>209</v>
       </c>
@@ -18774,8 +18863,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="38"/>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="43"/>
       <c r="B9" s="16" t="s">
         <v>640</v>
       </c>
@@ -18786,7 +18875,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="10" t="s">
         <v>212</v>
@@ -18798,8 +18887,8 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="39" t="s">
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
         <v>176</v>
       </c>
       <c r="B11" s="25" t="s">
@@ -18812,8 +18901,8 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="39"/>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="42"/>
       <c r="B12" s="10" t="s">
         <v>236</v>
       </c>
@@ -18824,8 +18913,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="39"/>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="42"/>
       <c r="B13" s="10" t="s">
         <v>243</v>
       </c>
@@ -18836,8 +18925,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="39"/>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="42"/>
       <c r="B14" s="25" t="s">
         <v>239</v>
       </c>
@@ -18848,13 +18937,13 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="39"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="42"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="14"/>
     </row>
-    <row r="16" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="B16" s="3" t="s">
         <v>218</v>
@@ -18866,8 +18955,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="38" t="s">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
         <v>175</v>
       </c>
       <c r="B17" s="25" t="s">
@@ -18880,8 +18969,8 @@
         <v>223</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="38"/>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="43"/>
       <c r="B18" s="13" t="s">
         <v>224</v>
       </c>
@@ -18892,8 +18981,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="38"/>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="43"/>
       <c r="B19" s="25" t="s">
         <v>227</v>
       </c>
@@ -18904,8 +18993,8 @@
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="38"/>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="43"/>
       <c r="B20" s="22" t="s">
         <v>544</v>
       </c>
@@ -18916,13 +19005,13 @@
         <v>545</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="38"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="43"/>
       <c r="B21" s="25"/>
       <c r="C21" s="6"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="22" t="s">
         <v>230</v>
       </c>
@@ -18933,8 +19022,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="39" t="s">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
         <v>246</v>
       </c>
       <c r="B23" s="22" t="s">
@@ -18947,8 +19036,8 @@
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="39"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -18972,19 +19061,19 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -18993,7 +19082,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>279</v>
       </c>
@@ -19002,7 +19091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>377</v>
       </c>
@@ -19013,7 +19102,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>378</v>
       </c>
@@ -19024,7 +19113,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>282</v>
       </c>
@@ -19035,7 +19124,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
         <v>285</v>
       </c>
@@ -19046,7 +19135,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>288</v>
       </c>
@@ -19057,7 +19146,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
         <v>291</v>
       </c>
@@ -19068,7 +19157,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>294</v>
       </c>
@@ -19079,7 +19168,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
         <v>297</v>
       </c>
@@ -19090,7 +19179,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
         <v>300</v>
       </c>
@@ -19101,7 +19190,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
         <v>303</v>
       </c>
@@ -19112,7 +19201,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
         <v>305</v>
       </c>
@@ -19123,7 +19212,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>308</v>
       </c>
@@ -19134,7 +19223,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
         <v>382</v>
       </c>
@@ -19145,7 +19234,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
         <v>406</v>
       </c>
@@ -19156,7 +19245,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="145" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" ht="165" x14ac:dyDescent="0.25">
       <c r="B19" s="22" t="s">
         <v>407</v>
       </c>
@@ -19167,7 +19256,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
         <v>381</v>
       </c>
@@ -19178,7 +19267,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
         <v>617</v>
       </c>
@@ -19207,19 +19296,19 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -19228,7 +19317,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>86</v>
       </c>
@@ -19237,7 +19326,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>247</v>
       </c>
@@ -19248,7 +19337,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>248</v>
       </c>
@@ -19259,7 +19348,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>580</v>
       </c>
@@ -19270,7 +19359,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>582</v>
       </c>
@@ -19281,7 +19370,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>586</v>
       </c>
@@ -19292,7 +19381,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>589</v>
       </c>
@@ -19303,7 +19392,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>312</v>
       </c>
@@ -19314,7 +19403,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>313</v>
       </c>
@@ -19325,7 +19414,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
         <v>591</v>
       </c>
@@ -19336,7 +19425,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>592</v>
       </c>
@@ -19347,7 +19436,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="16" t="s">
         <v>269</v>
       </c>
@@ -19358,7 +19447,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
         <v>270</v>
       </c>
@@ -19369,7 +19458,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
         <v>427</v>
       </c>
@@ -19380,7 +19469,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
         <v>429</v>
       </c>
@@ -19391,7 +19480,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="16" t="s">
         <v>432</v>
       </c>
@@ -19402,7 +19491,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="16" t="s">
         <v>434</v>
       </c>
@@ -19413,7 +19502,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="16" t="s">
         <v>439</v>
       </c>
@@ -19424,7 +19513,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
         <v>441</v>
       </c>
@@ -19435,7 +19524,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="16" t="s">
         <v>275</v>
       </c>
@@ -19446,7 +19535,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="s">
         <v>277</v>
       </c>
@@ -19457,7 +19546,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B25" s="16" t="s">
         <v>91</v>
       </c>
@@ -19468,7 +19557,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" s="16" t="s">
         <v>80</v>
       </c>
@@ -19479,7 +19568,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B27" s="16" t="s">
         <v>83</v>
       </c>
@@ -19490,7 +19579,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="s">
         <v>96</v>
       </c>
@@ -19519,19 +19608,19 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.6328125" customWidth="1"/>
-    <col min="4" max="4" width="46.6328125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="2:4" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>38</v>
       </c>
@@ -19540,7 +19629,7 @@
       </c>
       <c r="D2" s="35"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="36" t="s">
         <v>326</v>
       </c>
@@ -19549,7 +19638,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>327</v>
       </c>
@@ -19560,7 +19649,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>330</v>
       </c>
@@ -19571,7 +19660,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>333</v>
       </c>
@@ -19582,7 +19671,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>336</v>
       </c>
@@ -19593,7 +19682,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>352</v>
       </c>
@@ -19604,7 +19693,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>351</v>
       </c>
@@ -19615,7 +19704,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>356</v>
       </c>
@@ -19626,7 +19715,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>340</v>
       </c>
@@ -19635,12 +19724,12 @@
         <v>341</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="36" t="s">
         <v>367</v>
       </c>
@@ -19649,7 +19738,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
         <v>368</v>
       </c>
@@ -19660,7 +19749,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="87" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
         <v>371</v>
       </c>
@@ -19671,7 +19760,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>374</v>
       </c>

</xml_diff>